<commit_message>
Agregando la funcionalidad a las demas secciones
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Ciencias.xlsx
+++ b/app/src/main/assets/Ciencias.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\Llapanmi\app\src\main\res\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luigi\Documents\GitHub\llapanmi\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>ciencias;¿Cuál es la distribución de Linux más usada?;Ubunto;Debian;Fedora;Mint;</t>
   </si>
   <si>
-    <t>ciencias;¿Cómo llamamos a una lesión térmica o química de los tejidos?;Quemadura;Inflamación;Úlcera,Hernia;</t>
-  </si>
-  <si>
     <t>ciencias;¿Con qué nombre se conoce la energía producida por las partículas en movimiento?;Energía Cinética;Energía Solar;Energía Potencial;Energía Eólica;</t>
   </si>
   <si>
@@ -324,13 +321,16 @@
   </si>
   <si>
     <t>ciencias;¿Qué son los triglicéridos?;Lípidos;Glucidos;Proteínas;Vitaminas;Un triglicérido es un tipo de glicerol que pertenece a la familia de los lípidos y se forma por la esterificación de los tres grupos OH de los gliceroles por diferentes o igual tipo de ácidos grasos.</t>
+  </si>
+  <si>
+    <t>ciencias;¿Cómo llamamos a una lesión térmica o química de los tejidos?;Quemadura;Inflamación;Úlcera;Hernia;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +343,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,11 +387,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,12 +730,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -956,282 +969,282 @@
     </row>
     <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1241,7 +1254,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1253,7 +1266,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1265,6 +1278,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E0CF17DA3D1FD1438F9CF040CBCE9CAE" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="addee1f8e098277a732086128449e3a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1493ea5a-5927-4d40-8092-639a86616642" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e61f966c9f6e9aa2d131fd24b9b7016" ns2:_="">
     <xsd:import namespace="1493ea5a-5927-4d40-8092-639a86616642"/>
@@ -1408,12 +1427,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1424,6 +1437,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11B4FF55-1241-435C-A624-146B86EF8DD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B1E644A-AC99-44BB-81DE-D271E8BA7FD0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1441,15 +1463,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11B4FF55-1241-435C-A624-146B86EF8DD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E06AC9A9-F465-4361-99EC-3F360A35A3BB}">
   <ds:schemaRefs>

</xml_diff>